<commit_message>
v1.1 update reviewer verification status to closed
close registration wireframe review and verify the updates
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -64,9 +64,6 @@
     <t>v1.0</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>22/4/2025</t>
   </si>
   <si>
@@ -86,6 +83,15 @@
   </si>
   <si>
     <t>Initial version of review on registration wireframe</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>close registration wireframe review and verify the updates</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -337,12 +343,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -699,173 +699,173 @@
     <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="16" customFormat="1" ht="18.75">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="120">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>14</v>
+      <c r="H2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="22"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="30"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="19"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -886,7 +886,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -916,20 +916,28 @@
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="10">
         <v>45769</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="11"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+    <row r="3" spans="1:4" ht="37.5">
+      <c r="A3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="10">
+        <v>45770</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="8"/>

</xml_diff>

<commit_message>
v1.2 reopen registration wireframe registration
ask to add more details to registration form wireframe
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="4575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF_REGISTRATION_REVIEW" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>close registration wireframe review and verify the updates</t>
+  </si>
+  <si>
+    <t>LH_WF_REGISTRATION_REVIEW_002</t>
+  </si>
+  <si>
+    <t>27/4/2025</t>
+  </si>
+  <si>
+    <t>back to SRS I found there are many error messages for many validations like existing user name or existing email or validations fro password</t>
+  </si>
+  <si>
+    <t>so I prefer to add some error messages "with red color" from the SRS to wireframe to make it more expressive, you can back to login wireframe to understand what I mean</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>ask to add more details to registration form wireframe</t>
   </si>
 </sst>
 </file>
@@ -681,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -757,16 +778,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="20"/>
+    <row r="3" spans="1:9" ht="150">
+      <c r="A3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="28"/>
@@ -886,7 +925,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -939,11 +978,19 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="10">
+        <v>45774</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.3 Closed open reviews
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB077C65-DD91-4189-9745-771D5184E584}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="4575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF_REGISTRATION_REVIEW" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -113,12 +114,21 @@
   </si>
   <si>
     <t>ask to add more details to registration form wireframe</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed reviews </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -699,11 +709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -801,7 +811,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>28</v>
@@ -909,10 +919,10 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -921,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -992,6 +1002,20 @@
         <v>45774</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="18.75">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="10">
+        <v>45776</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.3 verify that the previous comments modified
close registration wireframe review, verify the updates and modify id naming convention
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_REGISTRATION_REVIEWS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB077C65-DD91-4189-9745-771D5184E584}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="4575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF_REGISTRATION_REVIEW" sheetId="3" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -68,9 +67,6 @@
     <t>22/4/2025</t>
   </si>
   <si>
-    <t>LH_WF_REGISTRATION_REVIEW_001</t>
-  </si>
-  <si>
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
@@ -95,9 +91,6 @@
     <t>close registration wireframe review and verify the updates</t>
   </si>
   <si>
-    <t>LH_WF_REGISTRATION_REVIEW_002</t>
-  </si>
-  <si>
     <t>27/4/2025</t>
   </si>
   <si>
@@ -107,9 +100,6 @@
     <t>so I prefer to add some error messages "with red color" from the SRS to wireframe to make it more expressive, you can back to login wireframe to understand what I mean</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>v1.2</t>
   </si>
   <si>
@@ -119,16 +109,19 @@
     <t>v1.3</t>
   </si>
   <si>
-    <t>Gehad Ashry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closed reviews </t>
+    <t>LH-WF-REGISTRATION-REVIEW-001</t>
+  </si>
+  <si>
+    <t>LH-WF-REGISTRATION-REVIEW-002</t>
+  </si>
+  <si>
+    <t>close registration wireframe review, verify the updates and modify id naming convention</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -709,11 +702,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -764,57 +757,57 @@
         <v>14</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="150">
       <c r="A3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -919,10 +912,10 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I12">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H12">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -931,11 +924,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C13" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,10 +958,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="10">
         <v>45769</v>
@@ -976,13 +969,13 @@
     </row>
     <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="10">
         <v>45770</v>
@@ -990,30 +983,30 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" s="10">
         <v>45774</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75">
+    <row r="5" spans="1:4" ht="56.25">
       <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="D5" s="10">
-        <v>45776</v>
+        <v>45775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>